<commit_message>
change in excel data
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/LoginData.xlsx
+++ b/src/test/resources/test-data/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\automation-workspace\automation-framework-ui-api\src\test\resources\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C73C69F-CFEA-45CE-848C-AD68022ABDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC5B93D-FF39-4D36-8858-26EBE5121584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>emailAddress</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>dpaul</t>
-  </si>
-  <si>
-    <t>abcdef</t>
   </si>
 </sst>
 </file>
@@ -354,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,14 +379,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="abc.def@test.com" xr:uid="{7FCE3EE1-B998-461A-812D-142233F7F1F2}"/>

</xml_diff>

<commit_message>
added api tests and changes in testng file
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/LoginData.xlsx
+++ b/src/test/resources/test-data/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\automation-workspace\automation-framework-ui-api\src\test\resources\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9074871-E425-4C85-B524-34FF8AFA5A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400BAFD7-1FCA-4F9D-8131-3E43AF16E29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>emailAddress</t>
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>dpaul</t>
   </si>
   <si>
     <t>abcdef</t>
@@ -354,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -382,18 +379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="abc.def@test.com" xr:uid="{7FCE3EE1-B998-461A-812D-142233F7F1F2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added parallel=true in dataprovider to resolve the remote execution failure
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/LoginData.xlsx
+++ b/src/test/resources/test-data/LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\automation-workspace\automation-framework-ui-api\src\test\resources\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400BAFD7-1FCA-4F9D-8131-3E43AF16E29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACF65C4-179C-4F13-9F42-F414C47105D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>emailAddress</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>abcdef</t>
+  </si>
+  <si>
+    <t>dpaul</t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,6 +382,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes in ui test
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/LoginData.xlsx
+++ b/src/test/resources/test-data/LoginData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\automation-workspace\automation-framework-ui-api\src\test\resources\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97878179-FB4D-41D4-A735-86131A81BBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60059040-4CD8-48FB-9C4F-26166D3BE1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
-    <t>emailAddress</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -37,6 +34,9 @@
   </si>
   <si>
     <t>dpaul</t>
+  </si>
+  <si>
+    <t>userName</t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -368,26 +368,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>